<commit_message>
Added column reordering and unit testing
</commit_message>
<xml_diff>
--- a/notedb/tests/test_files/test_tape_format_1.xlsx
+++ b/notedb/tests/test_files/test_tape_format_1.xlsx
@@ -64,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="00000"/>
+    <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -97,7 +97,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,24 +381,24 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -409,13 +409,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="1">
         <v>1844</v>
@@ -426,13 +426,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>17013</v>

</xml_diff>

<commit_message>
Tape can create Address and Note objects now
</commit_message>
<xml_diff>
--- a/notedb/tests/test_files/test_tape_format_1.xlsx
+++ b/notedb/tests/test_files/test_tape_format_1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayates\git\notedb\notedb\tests\test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey\git\notedb\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6036"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,18 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip</t>
-  </si>
-  <si>
     <t>BPO</t>
   </si>
   <si>
@@ -57,6 +45,18 @@
   </si>
   <si>
     <t>Pennslyvania</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>zipcode</t>
   </si>
 </sst>
 </file>
@@ -102,8 +102,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -381,41 +409,41 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="1">
         <v>1844</v>
@@ -424,15 +452,15 @@
         <v>410000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <v>17013</v>

</xml_diff>

<commit_message>
Added another unit test for Tape
</commit_message>
<xml_diff>
--- a/notedb/tests/test_files/test_tape_format_1.xlsx
+++ b/notedb/tests/test_files/test_tape_format_1.xlsx
@@ -44,9 +44,6 @@
     <t>Carlisle</t>
   </si>
   <si>
-    <t>Pennslyvania</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>zipcode</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
@@ -409,27 +409,27 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>

</xml_diff>